<commit_message>
Change slash direction in exception paths
</commit_message>
<xml_diff>
--- a/logic/test/data/spatialinventory/exceptions_spatial_disaggregation.xlsx
+++ b/logic/test/data/spatialinventory/exceptions_spatial_disaggregation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\spatialinventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E8E94F-E6BE-4BE7-AE53-60926E17704D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B753119-0537-46A0-9906-3EE07E88F6A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="5" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
@@ -1391,64 +1391,64 @@
     <t>Road transport: Resuspension</t>
   </si>
   <si>
-    <t>.\wegverkeer\2021\1A3BI_CO_2015.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BII_CO_2015.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIII_CO_2015.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIV_CO_2015.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BI_CO_2016.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BII_CO_2016.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIII_CO_2016.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIV_CO_2016.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BI_CO_2017.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BII_CO_2017.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIII_CO_2017.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIV_CO_2017.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BI_CO_2018.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BII_CO_2018.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIII_CO_2018.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIV_CO_2018.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BI_CO_2019.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BII_CO_2019.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIII_CO_2019.tif</t>
-  </si>
-  <si>
-    <t>.\wegverkeer\2021\1A3BIV_CO_2019.tif</t>
+    <t>./wegverkeer/2021/1A3BI_CO_2015.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BII_CO_2015.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIII_CO_2015.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIV_CO_2015.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BI_CO_2016.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BII_CO_2016.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIII_CO_2016.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIV_CO_2016.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BI_CO_2017.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BII_CO_2017.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIII_CO_2017.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIV_CO_2017.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BI_CO_2018.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BII_CO_2018.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIII_CO_2018.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIV_CO_2018.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BI_CO_2019.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BII_CO_2019.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIII_CO_2019.tif</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/1A3BIV_CO_2019.tif</t>
   </si>
 </sst>
 </file>
@@ -1574,6 +1574,168 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="47">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1934,168 +2096,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2172,38 +2172,38 @@
     <tableColumn id="4" xr3:uid="{98A5C858-28E9-44AB-8218-0A98439E4FDD}" name="GNFR_code"/>
     <tableColumn id="5" xr3:uid="{E012C600-87B4-47D1-9988-30D2C112D83D}" name="NFR_code"/>
     <tableColumn id="12" xr3:uid="{2155F8C1-A823-4717-B464-22F4A9A05E6A}" name="file_path"/>
-    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="46">
+    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="10">
       <calculatedColumnFormula>INDEX(tbl_country[country_label],MATCH(tbl_I_spatial_distribution[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="45">
+    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="9">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="8">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_spatial_distribution[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="6">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_spatial_distribution[[#This Row],[GNFR_code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[Year]]),"",tbl_I_spatial_distribution[[#This Row],[Year]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="40">
+    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[pollutant_code]]),"",tbl_I_spatial_distribution[[#This Row],[pollutant_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="39">
+    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[country_iso_code]]),"",tbl_I_spatial_distribution[[#This Row],[country_iso_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="38">
+    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_spatial_distribution[[#This Row],[GNFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="37">
+    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[NFR_code]]),"*",tbl_I_spatial_distribution[[#This Row],[NFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_file_path" dataDxfId="36">
+    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_file_path" dataDxfId="0">
       <calculatedColumnFormula>tbl_I_spatial_distribution[[#This Row],[file_path]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5303,7 +5303,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="Q2" s="3" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BI_CO_2015.tif</v>
+        <v>./wegverkeer/2021/1A3BI_CO_2015.tif</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="Q3" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BII_CO_2015.tif</v>
+        <v>./wegverkeer/2021/1A3BII_CO_2015.tif</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="Q4" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIII_CO_2015.tif</v>
+        <v>./wegverkeer/2021/1A3BIII_CO_2015.tif</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="Q5" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIV_CO_2015.tif</v>
+        <v>./wegverkeer/2021/1A3BIV_CO_2015.tif</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -5687,7 +5687,7 @@
       </c>
       <c r="Q6" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BI_CO_2016.tif</v>
+        <v>./wegverkeer/2021/1A3BI_CO_2016.tif</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -5749,7 +5749,7 @@
       </c>
       <c r="Q7" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BII_CO_2016.tif</v>
+        <v>./wegverkeer/2021/1A3BII_CO_2016.tif</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="Q8" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIII_CO_2016.tif</v>
+        <v>./wegverkeer/2021/1A3BIII_CO_2016.tif</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="Q9" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIV_CO_2016.tif</v>
+        <v>./wegverkeer/2021/1A3BIV_CO_2016.tif</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -5935,7 +5935,7 @@
       </c>
       <c r="Q10" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BI_CO_2017.tif</v>
+        <v>./wegverkeer/2021/1A3BI_CO_2017.tif</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="Q11" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BII_CO_2017.tif</v>
+        <v>./wegverkeer/2021/1A3BII_CO_2017.tif</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="Q12" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIII_CO_2017.tif</v>
+        <v>./wegverkeer/2021/1A3BIII_CO_2017.tif</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="Q13" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIV_CO_2017.tif</v>
+        <v>./wegverkeer/2021/1A3BIV_CO_2017.tif</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6183,7 +6183,7 @@
       </c>
       <c r="Q14" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BI_CO_2018.tif</v>
+        <v>./wegverkeer/2021/1A3BI_CO_2018.tif</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="Q15" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BII_CO_2018.tif</v>
+        <v>./wegverkeer/2021/1A3BII_CO_2018.tif</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="Q16" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIII_CO_2018.tif</v>
+        <v>./wegverkeer/2021/1A3BIII_CO_2018.tif</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -6369,7 +6369,7 @@
       </c>
       <c r="Q17" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIV_CO_2018.tif</v>
+        <v>./wegverkeer/2021/1A3BIV_CO_2018.tif</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -6431,7 +6431,7 @@
       </c>
       <c r="Q18" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BI_CO_2019.tif</v>
+        <v>./wegverkeer/2021/1A3BI_CO_2019.tif</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -6493,7 +6493,7 @@
       </c>
       <c r="Q19" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BII_CO_2019.tif</v>
+        <v>./wegverkeer/2021/1A3BII_CO_2019.tif</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -6555,7 +6555,7 @@
       </c>
       <c r="Q20" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIII_CO_2019.tif</v>
+        <v>./wegverkeer/2021/1A3BIII_CO_2019.tif</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -6617,188 +6617,188 @@
       </c>
       <c r="Q21" s="8" t="str">
         <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
-        <v>.\wegverkeer\2021\1A3BIV_CO_2019.tif</v>
+        <v>./wegverkeer/2021/1A3BIV_CO_2019.tif</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="35" priority="883">
+    <cfRule type="expression" dxfId="46" priority="883">
       <formula>$K2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F21 A2:C21">
-    <cfRule type="expression" dxfId="34" priority="882">
+    <cfRule type="expression" dxfId="45" priority="882">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="33" priority="881">
+    <cfRule type="expression" dxfId="44" priority="881">
       <formula>$K3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C3 F3">
-    <cfRule type="expression" dxfId="32" priority="880">
+    <cfRule type="expression" dxfId="43" priority="880">
       <formula>ISBLANK(A3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="31" priority="879">
+    <cfRule type="expression" dxfId="42" priority="879">
       <formula>$K4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4 F4">
-    <cfRule type="expression" dxfId="30" priority="878">
+    <cfRule type="expression" dxfId="41" priority="878">
       <formula>ISBLANK(A4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="29" priority="877">
+    <cfRule type="expression" dxfId="40" priority="877">
       <formula>$K5=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C5 F5">
-    <cfRule type="expression" dxfId="28" priority="876">
+    <cfRule type="expression" dxfId="39" priority="876">
       <formula>ISBLANK(A5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:C9 F6:F9">
-    <cfRule type="expression" dxfId="27" priority="875">
+    <cfRule type="expression" dxfId="38" priority="875">
       <formula>ISBLANK(A6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="26" priority="874">
+    <cfRule type="expression" dxfId="37" priority="874">
       <formula>$K7=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C7 F7">
-    <cfRule type="expression" dxfId="25" priority="873">
+    <cfRule type="expression" dxfId="36" priority="873">
       <formula>ISBLANK(A7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="24" priority="872">
+    <cfRule type="expression" dxfId="35" priority="872">
       <formula>$K8=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 F8">
-    <cfRule type="expression" dxfId="23" priority="871">
+    <cfRule type="expression" dxfId="34" priority="871">
       <formula>ISBLANK(A8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="22" priority="870">
+    <cfRule type="expression" dxfId="33" priority="870">
       <formula>$K9=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:C9 F9">
-    <cfRule type="expression" dxfId="21" priority="869">
+    <cfRule type="expression" dxfId="32" priority="869">
       <formula>ISBLANK(A9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:C13 F10:F13">
-    <cfRule type="expression" dxfId="20" priority="868">
+    <cfRule type="expression" dxfId="31" priority="868">
       <formula>ISBLANK(A10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="19" priority="867">
+    <cfRule type="expression" dxfId="30" priority="867">
       <formula>$K11=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:C11 F11">
-    <cfRule type="expression" dxfId="18" priority="866">
+    <cfRule type="expression" dxfId="29" priority="866">
       <formula>ISBLANK(A11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="17" priority="865">
+    <cfRule type="expression" dxfId="28" priority="865">
       <formula>$K12=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:C12 F12">
-    <cfRule type="expression" dxfId="16" priority="864">
+    <cfRule type="expression" dxfId="27" priority="864">
       <formula>ISBLANK(A12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="15" priority="863">
+    <cfRule type="expression" dxfId="26" priority="863">
       <formula>$K13=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:C13 F13">
-    <cfRule type="expression" dxfId="14" priority="862">
+    <cfRule type="expression" dxfId="25" priority="862">
       <formula>ISBLANK(A13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:C17 F14:F17">
-    <cfRule type="expression" dxfId="13" priority="861">
+    <cfRule type="expression" dxfId="24" priority="861">
       <formula>ISBLANK(A14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="12" priority="860">
+    <cfRule type="expression" dxfId="23" priority="860">
       <formula>$K15=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C15 F15">
-    <cfRule type="expression" dxfId="11" priority="859">
+    <cfRule type="expression" dxfId="22" priority="859">
       <formula>ISBLANK(A15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="10" priority="858">
+    <cfRule type="expression" dxfId="21" priority="858">
       <formula>$K16=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:C16 F16">
-    <cfRule type="expression" dxfId="9" priority="857">
+    <cfRule type="expression" dxfId="20" priority="857">
       <formula>ISBLANK(A16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="8" priority="856">
+    <cfRule type="expression" dxfId="19" priority="856">
       <formula>$K17=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:C17 F17">
-    <cfRule type="expression" dxfId="7" priority="855">
+    <cfRule type="expression" dxfId="18" priority="855">
       <formula>ISBLANK(A17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:C21 F18:F21">
-    <cfRule type="expression" dxfId="6" priority="854">
+    <cfRule type="expression" dxfId="17" priority="854">
       <formula>ISBLANK(A18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="5" priority="853">
+    <cfRule type="expression" dxfId="16" priority="853">
       <formula>$K19=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:C19 F19">
-    <cfRule type="expression" dxfId="4" priority="852">
+    <cfRule type="expression" dxfId="15" priority="852">
       <formula>ISBLANK(A19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="3" priority="851">
+    <cfRule type="expression" dxfId="14" priority="851">
       <formula>$K20=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:C20 F20">
-    <cfRule type="expression" dxfId="2" priority="850">
+    <cfRule type="expression" dxfId="13" priority="850">
       <formula>ISBLANK(A20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="1" priority="849">
+    <cfRule type="expression" dxfId="12" priority="849">
       <formula>$K21=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:C21 F21">
-    <cfRule type="expression" dxfId="0" priority="848">
+    <cfRule type="expression" dxfId="11" priority="848">
       <formula>ISBLANK(A21)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed nodata issue when warping rasters
</commit_message>
<xml_diff>
--- a/logic/test/data/spatialinventory/exceptions_spatial_disaggregation.xlsx
+++ b/logic/test/data/spatialinventory/exceptions_spatial_disaggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\spatialinventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D18855-D59F-4646-AA76-8C11D8D1274C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3DA0CE-792D-4750-B99F-DE97DC8173BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-110" windowWidth="37670" windowHeight="21820" activeTab="5" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" activeTab="5" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
   <sheets>
     <sheet name="GNFR" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="466">
   <si>
     <t>A_PublicPower</t>
   </si>
@@ -1461,6 +1461,9 @@
   </si>
   <si>
     <t>via_GNFR</t>
+  </si>
+  <si>
+    <t>./wegverkeer/2021/B_Industry_CO_2019.tif</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1588,169 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1948,165 +2113,53 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2187,38 +2240,38 @@
     <tableColumn id="2" xr3:uid="{34470E06-D53A-4CB8-883D-67C79F759C3B}" name="type"/>
     <tableColumn id="14" xr3:uid="{F12554B4-D21C-46BF-A7E1-572FE2F30F2C}" name="via_NFR"/>
     <tableColumn id="20" xr3:uid="{45D262D2-7868-46E7-AB75-B5A5A94061E0}" name="via_GNFR"/>
-    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="46">
+    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="10">
       <calculatedColumnFormula>INDEX(tbl_country[country_label],MATCH(tbl_I_spatial_distribution[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="45">
+    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="9">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="8">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_spatial_distribution[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="6">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_spatial_distribution[[#This Row],[GNFR_code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[Year]]),"",tbl_I_spatial_distribution[[#This Row],[Year]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="40">
+    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[pollutant_code]]),"",tbl_I_spatial_distribution[[#This Row],[pollutant_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="39">
+    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[country_iso_code]]),"",tbl_I_spatial_distribution[[#This Row],[country_iso_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="38">
+    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_spatial_distribution[[#This Row],[GNFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="37">
+    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[NFR_code]]),"*",tbl_I_spatial_distribution[[#This Row],[NFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_file_path" dataDxfId="36">
+    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_file_path" dataDxfId="0">
       <calculatedColumnFormula>tbl_I_spatial_distribution[[#This Row],[file_path]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5315,10 +5368,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6707,199 +6760,289 @@
         <v>./wegverkeer/2021/1A3BIV_CO_2019.tif</v>
       </c>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2016</v>
+      </c>
+      <c r="B22" t="s">
+        <v>396</v>
+      </c>
+      <c r="C22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" t="s">
+        <v>465</v>
+      </c>
+      <c r="G22" t="s">
+        <v>462</v>
+      </c>
+      <c r="J22" s="1" t="e">
+        <f>INDEX(tbl_country[country_label],MATCH(tbl_I_spatial_distribution[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="7" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L22" s="1" t="e">
+        <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M22" s="8" t="str">
+        <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_spatial_distribution[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_spatial_distribution[[#This Row],[GNFR_code]])),
+_xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
+        <v>'GNFR-NFR'!C2:C129</v>
+      </c>
+      <c r="N22" s="3" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_spatial_distribution[[#This Row],[GNFR_code]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O22" s="8" t="e">
+        <f>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[Year]]),"",tbl_I_spatial_distribution[[#This Row],[Year]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P22" s="8" t="e">
+        <f>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[pollutant_code]]),"",tbl_I_spatial_distribution[[#This Row],[pollutant_code]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q22" s="8" t="e">
+        <f>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[country_iso_code]]),"",tbl_I_spatial_distribution[[#This Row],[country_iso_code]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R22" s="8" t="e">
+        <f>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_spatial_distribution[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_spatial_distribution[[#This Row],[GNFR_code]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S22" s="8" t="e">
+        <f>IF(ISBLANK(tbl_I_spatial_distribution[[#This Row],[NFR_code]]),"*",tbl_I_spatial_distribution[[#This Row],[NFR_code]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T22" s="8" t="e">
+        <f>tbl_I_spatial_distribution[[#This Row],[file_path]]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="35" priority="883">
+    <cfRule type="expression" dxfId="51" priority="888">
       <formula>$N2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:C21 F2:I21">
-    <cfRule type="expression" dxfId="34" priority="882">
+    <cfRule type="expression" dxfId="50" priority="887">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="33" priority="881">
+    <cfRule type="expression" dxfId="49" priority="886">
       <formula>$N3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C3 F3:I3">
-    <cfRule type="expression" dxfId="32" priority="880">
+    <cfRule type="expression" dxfId="48" priority="885">
       <formula>ISBLANK(A3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="31" priority="879">
+    <cfRule type="expression" dxfId="47" priority="884">
       <formula>$N4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4 F4:I4">
-    <cfRule type="expression" dxfId="30" priority="878">
+    <cfRule type="expression" dxfId="46" priority="883">
       <formula>ISBLANK(A4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="29" priority="877">
+    <cfRule type="expression" dxfId="45" priority="882">
       <formula>$N5=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C5 F5:I5">
-    <cfRule type="expression" dxfId="28" priority="876">
+    <cfRule type="expression" dxfId="44" priority="881">
       <formula>ISBLANK(A5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:C9 F6:I9">
-    <cfRule type="expression" dxfId="27" priority="875">
+    <cfRule type="expression" dxfId="43" priority="880">
       <formula>ISBLANK(A6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="26" priority="874">
+    <cfRule type="expression" dxfId="42" priority="879">
       <formula>$N7=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C7 F7:I7">
-    <cfRule type="expression" dxfId="25" priority="873">
+    <cfRule type="expression" dxfId="41" priority="878">
       <formula>ISBLANK(A7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="24" priority="872">
+    <cfRule type="expression" dxfId="40" priority="877">
       <formula>$N8=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 F8:I8">
-    <cfRule type="expression" dxfId="23" priority="871">
+    <cfRule type="expression" dxfId="39" priority="876">
       <formula>ISBLANK(A8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="22" priority="870">
+    <cfRule type="expression" dxfId="38" priority="875">
       <formula>$N9=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:C9 F9:I9">
-    <cfRule type="expression" dxfId="21" priority="869">
+    <cfRule type="expression" dxfId="37" priority="874">
       <formula>ISBLANK(A9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:C13 F10:I13">
-    <cfRule type="expression" dxfId="20" priority="868">
+    <cfRule type="expression" dxfId="36" priority="873">
       <formula>ISBLANK(A10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="19" priority="867">
+    <cfRule type="expression" dxfId="35" priority="872">
       <formula>$N11=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:C11 F11:I11">
-    <cfRule type="expression" dxfId="18" priority="866">
+    <cfRule type="expression" dxfId="34" priority="871">
       <formula>ISBLANK(A11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="17" priority="865">
+    <cfRule type="expression" dxfId="33" priority="870">
       <formula>$N12=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:C12 F12:I12">
-    <cfRule type="expression" dxfId="16" priority="864">
+    <cfRule type="expression" dxfId="32" priority="869">
       <formula>ISBLANK(A12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="15" priority="863">
+    <cfRule type="expression" dxfId="31" priority="868">
       <formula>$N13=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:C13 F13:I13">
-    <cfRule type="expression" dxfId="14" priority="862">
+    <cfRule type="expression" dxfId="30" priority="867">
       <formula>ISBLANK(A13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:C17 F14:I17">
-    <cfRule type="expression" dxfId="13" priority="861">
+    <cfRule type="expression" dxfId="29" priority="866">
       <formula>ISBLANK(A14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="12" priority="860">
+    <cfRule type="expression" dxfId="28" priority="865">
       <formula>$N15=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C15 F15:I15">
-    <cfRule type="expression" dxfId="11" priority="859">
+    <cfRule type="expression" dxfId="27" priority="864">
       <formula>ISBLANK(A15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="10" priority="858">
+    <cfRule type="expression" dxfId="26" priority="863">
       <formula>$N16=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:C16 F16:I16">
-    <cfRule type="expression" dxfId="9" priority="857">
+    <cfRule type="expression" dxfId="25" priority="862">
       <formula>ISBLANK(A16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="8" priority="856">
+    <cfRule type="expression" dxfId="24" priority="861">
       <formula>$N17=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:C17 F17:I17">
-    <cfRule type="expression" dxfId="7" priority="855">
+    <cfRule type="expression" dxfId="23" priority="860">
       <formula>ISBLANK(A17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:C21 F18:I21">
-    <cfRule type="expression" dxfId="6" priority="854">
+    <cfRule type="expression" dxfId="22" priority="859">
       <formula>ISBLANK(A18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="5" priority="853">
+    <cfRule type="expression" dxfId="21" priority="858">
       <formula>$N19=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:C19 F19:I19">
-    <cfRule type="expression" dxfId="4" priority="852">
+    <cfRule type="expression" dxfId="20" priority="857">
       <formula>ISBLANK(A19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="3" priority="851">
+    <cfRule type="expression" dxfId="19" priority="856">
       <formula>$N20=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:C20 F20:I20">
-    <cfRule type="expression" dxfId="2" priority="850">
+    <cfRule type="expression" dxfId="18" priority="855">
       <formula>ISBLANK(A20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="1" priority="849">
+    <cfRule type="expression" dxfId="17" priority="854">
       <formula>$N21=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:C21 F21:I21">
-    <cfRule type="expression" dxfId="0" priority="848">
+    <cfRule type="expression" dxfId="16" priority="853">
       <formula>ISBLANK(A21)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="expression" dxfId="15" priority="5">
+      <formula>$N22=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:C22 F22:I22">
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>ISBLANK(A22)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:C22 F22:I22">
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>ISBLANK(A22)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>$N22=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:C22 F22:I22">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>ISBLANK(A22)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B21" xr:uid="{408D5B29-ED64-41D6-B2C9-87834CC0D1A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22" xr:uid="{408D5B29-ED64-41D6-B2C9-87834CC0D1A5}">
       <formula1>pollutant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21" xr:uid="{3F75D6D0-D85E-4B43-9850-03184E40FE92}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C22" xr:uid="{3F75D6D0-D85E-4B43-9850-03184E40FE92}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{535DD205-1625-4419-AFA4-BB88C9609505}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D22" xr:uid="{535DD205-1625-4419-AFA4-BB88C9609505}">
       <formula1>GNFR</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{CFB1DFB7-1A2B-4733-8808-6A363CB09CD7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22" xr:uid="{CFB1DFB7-1A2B-4733-8808-6A363CB09CD7}">
       <formula1>INDIRECT(M2)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>